<commit_message>
Updated New Cartridge Changes
Updated New Cartridge Changes. These changes include newly done Passowrd reset implementation.
</commit_message>
<xml_diff>
--- a/documentation/SFCC_PRIOS_Integration_Test_Cases.xlsx
+++ b/documentation/SFCC_PRIOS_Integration_Test_Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -203,6 +203,48 @@
   </si>
   <si>
     <t>On search form the search box or on click of sub categories form the menu.</t>
+  </si>
+  <si>
+    <t>TC_ResettingCustomer'sPassword_001</t>
+  </si>
+  <si>
+    <t>Hit "Starts a password reset process" API by passing the identification and type in the body along with the OAuth Bearer token.</t>
+  </si>
+  <si>
+    <t>TC_ResettingCustomer'sPassword_002</t>
+  </si>
+  <si>
+    <t>To Update the password of the customer.</t>
+  </si>
+  <si>
+    <t>Generate JWT token so that it can used to update the password of the customer.</t>
+  </si>
+  <si>
+    <t>Hit "Update customer's password" API by passing the customerID in the URL and passing the current password and new password in the body along with the JWT Bearer token.</t>
+  </si>
+  <si>
+    <t>An email is sent to respective mail ID that is passed as identification parameter in the body of the API that contains the link that contains the form to change the password.</t>
+  </si>
+  <si>
+    <t>An email will be sent to respective mail ID that is passed with identification parameter in the body of the API that contains the link which contains the form to change the password.</t>
+  </si>
+  <si>
+    <t>The password of the customer is changed successfully.</t>
+  </si>
+  <si>
+    <t>The password of the customer has to be changed successfully</t>
+  </si>
+  <si>
+    <t>Starts a password reset process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update customer's password </t>
+  </si>
+  <si>
+    <t>To send an email to customer who wants to change the password.</t>
+  </si>
+  <si>
+    <t>Generate OAuth token so that it can be used to start the password reset process API.</t>
   </si>
 </sst>
 </file>
@@ -232,7 +274,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,8 +287,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -254,22 +302,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,11 +639,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -591,57 +657,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -649,28 +715,28 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -678,28 +744,28 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I4" s="3" t="s">
@@ -707,28 +773,28 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="3" t="s">
         <v>34</v>
       </c>
       <c r="I5" s="3" t="s">
@@ -736,28 +802,28 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I6" s="3" t="s">
@@ -765,28 +831,28 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I7" s="3" t="s">
@@ -794,28 +860,28 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="I8" s="3" t="s">
@@ -823,28 +889,28 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="3" t="s">
         <v>38</v>
       </c>
       <c r="I9" s="3" t="s">
@@ -852,28 +918,28 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>40</v>
       </c>
       <c r="I10" s="3" t="s">
@@ -881,31 +947,89 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="3" t="s">
         <v>42</v>
       </c>
       <c r="I11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>